<commit_message>
update manuscript and figures
</commit_message>
<xml_diff>
--- a/tables/Symbiont_proteomics.xlsx
+++ b/tables/Symbiont_proteomics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yzl0084/Documents/Research/Lamellibrachia-genome/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4497A5E3-B71E-6540-B7F1-09FFDED905BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBACE48-A142-BA40-872B-69D10BCF1D31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="3080" windowWidth="31960" windowHeight="16940" xr2:uid="{55004462-A508-4442-A1CD-C226A07D16A6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{55004462-A508-4442-A1CD-C226A07D16A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2812,12 +2812,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEAE787-8960-7B43-B7D1-8587999CB403}">
   <dimension ref="A1:L296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
       <selection activeCell="A271" activeCellId="27" sqref="A15:XFD15 A24:XFD24 A25:XFD25 A65:XFD65 A75:XFD75 A79:XFD79 A80:XFD80 A99:XFD99 A100:XFD100 A152:XFD152 A174:XFD174 A180:XFD180 A181:XFD181 A223:XFD223 A230:XFD230 A232:XFD232 A233:XFD233 A234:XFD234 A236:XFD236 A239:XFD239 A249:XFD249 A250:XFD250 A251:XFD251 A257:XFD257 A258:XFD258 A260:XFD260 A264:XFD264 A271:XFD271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="135.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="220" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>